<commit_message>
Add more positive cases for add stories, add negative cases for add stories and attach screenshots for design and execution
</commit_message>
<xml_diff>
--- a/High Level Scenarios FB.xlsx
+++ b/High Level Scenarios FB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aya\Egy FWD\Mobile app testing\MobileApplicationTesting-Facebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9208CC-8706-4537-B9B7-513D180E750C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900D8DB6-72AD-433B-B93D-51ECDF9FD22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="844" activeTab="3" xr2:uid="{5A6BC087-F653-4ABA-AD0D-CDE97249D429}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1776" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2498" uniqueCount="1036">
   <si>
     <t>Test Scenarios</t>
   </si>
@@ -2672,6 +2672,804 @@
   </si>
   <si>
     <t>Adding Stories | Positive test cases</t>
+  </si>
+  <si>
+    <t>Adding Stories | Negative test cases</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-1</t>
+  </si>
+  <si>
+    <t>Validate adding a story with no internet connection</t>
+  </si>
+  <si>
+    <t>Validate uploading a photo to a story without internet connection</t>
+  </si>
+  <si>
+    <t>Check UI when trying to add a story with text that includes very long words</t>
+  </si>
+  <si>
+    <t>Validate saving a story to phone</t>
+  </si>
+  <si>
+    <t>Check if you can see the story viewers within 24 hours after adding the story</t>
+  </si>
+  <si>
+    <t>Check if you can see the story viewers after 24 hours after adding the story</t>
+  </si>
+  <si>
+    <t>Validate tagging a blocked friend in a story</t>
+  </si>
+  <si>
+    <t>Validate tagging a deactivated account in a story</t>
+  </si>
+  <si>
+    <t>Validate adding a story with only a link</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and uploaded photo from the gallery</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and stickers</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and GIFs</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-31</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-32</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-33</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-34</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-35</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-36</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-37</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-38</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-39</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-40</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-41</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-42</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-43</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-44</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-45</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-46</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-47</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-48</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-49</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-50</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-51</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-52</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-53</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-54</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-55</t>
+  </si>
+  <si>
+    <t>Validate adding a story with stickers and GIFs</t>
+  </si>
+  <si>
+    <t>Validate adding a story with photo and stickers</t>
+  </si>
+  <si>
+    <t>Validate adding a story with photo and GIFs</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and video</t>
+  </si>
+  <si>
+    <t>Validate adding a story with GIF and video</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and a location</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and sound</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and green screen</t>
+  </si>
+  <si>
+    <t>Validate adding a story with stickers and video</t>
+  </si>
+  <si>
+    <t>Validate adding a story with stickers and location</t>
+  </si>
+  <si>
+    <t>Validate adding a story with stickers and sound</t>
+  </si>
+  <si>
+    <t>Validate adding a story with stickers and green screen</t>
+  </si>
+  <si>
+    <t>Validate adding a story with GIF and location</t>
+  </si>
+  <si>
+    <t>Validate adding a story with GIF and sound</t>
+  </si>
+  <si>
+    <t>Validate adding a story with GIF and boomerang</t>
+  </si>
+  <si>
+    <t>Validate adding a story with GIF and green screen</t>
+  </si>
+  <si>
+    <t>Validate adding a story with location and video</t>
+  </si>
+  <si>
+    <t>Validate adding a story with video and sound</t>
+  </si>
+  <si>
+    <t>Validate adding a story with video and boomerang</t>
+  </si>
+  <si>
+    <t>Validate adding a story with video and green screen</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-56</t>
+  </si>
+  <si>
+    <t>Validate adding a story with location and sound</t>
+  </si>
+  <si>
+    <t>validate adding a story with location and boomerang</t>
+  </si>
+  <si>
+    <t>validate adding a story with location and green screen</t>
+  </si>
+  <si>
+    <t>validate adding a story with location and photo</t>
+  </si>
+  <si>
+    <t>validate adding a story with sound and boomerang</t>
+  </si>
+  <si>
+    <t>validate adding a story with sound and photo</t>
+  </si>
+  <si>
+    <t>validate adding a story with sound and green screen</t>
+  </si>
+  <si>
+    <t>Validate adding effects to a story</t>
+  </si>
+  <si>
+    <t>Validate drawing free lines on a story</t>
+  </si>
+  <si>
+    <t>validate adding a question on a story</t>
+  </si>
+  <si>
+    <t>validate adding an event on a story</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-57</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-58</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-59</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-60</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-61</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-62</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-63</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-64</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-65</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-66</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-67</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Positive-68</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with text only</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a video</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a GIF</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a sticker</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with multiple GIFs and stickers</t>
+  </si>
+  <si>
+    <t>Validate deleting a story with friends tagged in it</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a photo</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a boomerang</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a sound</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a location</t>
+  </si>
+  <si>
+    <t>Validate deleting an already existing story with a green screen</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-2</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-3</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-4</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-5</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-6</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-7</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-8</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-9</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-10</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-11</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-12</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-13</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-14</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-15</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-16</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-17</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-18</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-19</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-20</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-21</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-22</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-23</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-24</t>
+  </si>
+  <si>
+    <t>Facebook-AddStory-Negative-25</t>
+  </si>
+  <si>
+    <t>Validate deleting a story after sharing it with a friend as a link</t>
+  </si>
+  <si>
+    <t>Validate deleting a story from a collection</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. upload photo from gallery
+3. add text
+4. add story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. click on camera icon
+3. capture a photo
+4. add text
+5. add them to story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add video
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add a GIF
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add GIF
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add a photo
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add location
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add video
+3. add GIF
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add location
+3. add video
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add boomerang
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add sound
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add video
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add text
+3. add green screen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add location
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add sound
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add boomerang
+3. add stickers
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add stickers
+3. add green screen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add GIF
+3. add green screen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add boomerang
+3. add green screen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add sound
+3. add green screen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add sound
+3. add GIF
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add GIF
+3. add location
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add video
+3. add sound
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add video
+3. add boomerang
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add video
+3. add greenscreen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add location
+3. add sound
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add location
+3. add boomerang
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add location
+3. add photo
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add location
+3. add green screen
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add sound
+3. add photo
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add sound
+3. add boomerang
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add a poll
+3. add a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add effects
+3. add a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add a question
+3. add a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add an event
+3. add a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. draw lines
+3. add a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add a story without internet</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add photo to a story without internet</t>
+  </si>
+  <si>
+    <t>1. a story should not be added</t>
+  </si>
+  <si>
+    <t>1. a story is not added</t>
+  </si>
+  <si>
+    <t>Validate sending a story in messenger</t>
+  </si>
+  <si>
+    <t>Validate deleting a story after adding it</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and uploaded photo from the Camera</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add photo
+3. add GIF
+4. add them to a story</t>
+  </si>
+  <si>
+    <t>Validate adding a story with text and boomerang</t>
+  </si>
+  <si>
+    <t>Validate adding a story with stickers and boomerang</t>
+  </si>
+  <si>
+    <t>Validate adding a poll to a story</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. write Germany sentences with very long words
+3. check UI</t>
+  </si>
+  <si>
+    <t>1. text should be wrapped and should not go out of the story frame</t>
+  </si>
+  <si>
+    <t>1. text is not wrapped and does not go out of the story frame</t>
+  </si>
+  <si>
+    <t>1. user should have an already added story</t>
+  </si>
+  <si>
+    <t>1. open a story
+2. click on the 3 dots menu
+3. copy story link
+4. send it to a friend
+5. check that a story can be shared</t>
+  </si>
+  <si>
+    <t>1. a story can be shared as a message</t>
+  </si>
+  <si>
+    <t>1. a story is shared as a message</t>
+  </si>
+  <si>
+    <t>1. open a story
+2. click on the 3 dots menu
+3. click on save to phone
+4. check gallery</t>
+  </si>
+  <si>
+    <t>1. story should be saved to phone</t>
+  </si>
+  <si>
+    <t>1. story is saved to phone</t>
+  </si>
+  <si>
+    <t>1. delete a story</t>
+  </si>
+  <si>
+    <t>1. a story should be deleted</t>
+  </si>
+  <si>
+    <t>1. a story is deleted</t>
+  </si>
+  <si>
+    <t>1. a story should be added within 24 hours</t>
+  </si>
+  <si>
+    <t>1. check that others can see the story</t>
+  </si>
+  <si>
+    <t>1. a story should remain visible to others within 24 hours</t>
+  </si>
+  <si>
+    <t>1. a story is visible to others within 24 hours</t>
+  </si>
+  <si>
+    <t>1. a story should be added 2 days ago</t>
+  </si>
+  <si>
+    <t>1. check if a story is visible</t>
+  </si>
+  <si>
+    <t>1. a story should be already added</t>
+  </si>
+  <si>
+    <t>Check story visibility adding it to a collection</t>
+  </si>
+  <si>
+    <t>1. add a story to a collection
+2. check story visibility</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. try tagging an account you blocked</t>
+  </si>
+  <si>
+    <t>1. user should not be able to tag blocked accounts</t>
+  </si>
+  <si>
+    <t>1. user is not able to tag blocked accounts</t>
+  </si>
+  <si>
+    <t>1. user should not be able to tag deactivated accounts</t>
+  </si>
+  <si>
+    <t>1. user is not able to tag deactivated accounts</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. add a link to a story
+3. post a story</t>
+  </si>
+  <si>
+    <t>1. a story with text only should be added</t>
+  </si>
+  <si>
+    <t>1. a story with video only should be added</t>
+  </si>
+  <si>
+    <t>1. a story with GIF should be added</t>
+  </si>
+  <si>
+    <t>1. a story with stickers should be added</t>
+  </si>
+  <si>
+    <t>1. a story with photo should be added</t>
+  </si>
+  <si>
+    <t>1. a story with boomerang should be added</t>
+  </si>
+  <si>
+    <t>1. a story with sound should be added</t>
+  </si>
+  <si>
+    <t>1. a story with location should be added</t>
+  </si>
+  <si>
+    <t>1. a story with green screen should be added</t>
+  </si>
+  <si>
+    <t>1. a story with a friend tagged in it should be added</t>
+  </si>
+  <si>
+    <t>1. a story linked should be already shared with a friend</t>
+  </si>
+  <si>
+    <t>1. a story should be already added to a collection</t>
+  </si>
+  <si>
+    <t>1. delete a story with friends tagged in it</t>
+  </si>
+  <si>
+    <t>1. delete a story after sharing its link with a friend</t>
+  </si>
+  <si>
+    <t>1. a story with GIFs and stickers should be added</t>
+  </si>
+  <si>
+    <t>1. delete a story from a collection</t>
+  </si>
+  <si>
+    <t>1. a story should not be visible after adding it with 24 hours</t>
+  </si>
+  <si>
+    <t>1. a story is not visible after adding it with 24 hours</t>
+  </si>
+  <si>
+    <t>1. a story should remain visible forever</t>
+  </si>
+  <si>
+    <t>1. a story is visible forever</t>
+  </si>
+  <si>
+    <t>1. click on story icon
+2. try tagging an account that is already deactivated</t>
+  </si>
+  <si>
+    <t>1. a story should be deleted from friend's side too</t>
+  </si>
+  <si>
+    <t>1. a story is deleted from friend's side too</t>
+  </si>
+  <si>
+    <t>1. story link should not be opened</t>
+  </si>
+  <si>
+    <t>1. story link is not opened</t>
+  </si>
+  <si>
+    <t>1. a story should be deleted from a collection</t>
+  </si>
+  <si>
+    <t>1. a story is deleted from a collection</t>
+  </si>
+  <si>
+    <t>medium</t>
   </si>
 </sst>
 </file>
@@ -3042,19 +3840,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4259,9 +5057,9 @@
   <dimension ref="A1:L123"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A91" sqref="A91:XFD91"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C86" sqref="C86"/>
+      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -7150,7 +7948,7 @@
       <c r="K91" s="34"/>
       <c r="L91" s="35"/>
     </row>
-    <row r="92" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:12" ht="99.6" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>336</v>
       </c>
@@ -7182,7 +7980,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12" ht="109.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>336</v>
       </c>
@@ -8134,22 +8932,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3687F5AB-AE89-403A-8C8A-0966CFB97A23}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="53.77734375" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
-    <col min="6" max="6" width="24.109375" customWidth="1"/>
-    <col min="7" max="7" width="32.109375" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" customWidth="1"/>
-    <col min="11" max="11" width="39.109375" customWidth="1"/>
-    <col min="12" max="12" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="44"/>
+    <col min="2" max="2" width="27.77734375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="53.77734375" style="19" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" style="44" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" style="44" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" style="44" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" style="44" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="44"/>
+    <col min="11" max="11" width="39.109375" style="44" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" style="44" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="21" customFormat="1" ht="21" x14ac:dyDescent="0.3">
@@ -8191,20 +8996,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="32" t="s">
         <v>577</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" s="19" customFormat="1" ht="158.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
@@ -8335,732 +9140,3009 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="32" customFormat="1" ht="18" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="32" t="s">
         <v>579</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="31"/>
-    </row>
-    <row r="8" spans="1:12" s="36" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+    </row>
+    <row r="8" spans="1:12" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
         <v>811</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35"/>
-    </row>
-    <row r="9" spans="1:12" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="45" t="s">
+    </row>
+    <row r="9" spans="1:12" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="43" t="s">
         <v>713</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="19" t="s">
         <v>580</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="19" t="s">
         <v>792</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="H9" s="44" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="45" t="s">
+      <c r="I9" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="43" t="s">
         <v>714</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="19" t="s">
         <v>581</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="19" t="s">
         <v>743</v>
       </c>
-      <c r="G10" s="45" t="s">
+      <c r="G10" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="45" t="s">
+      <c r="I10" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J10" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="43" t="s">
         <v>715</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="19" t="s">
         <v>793</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="19" t="s">
         <v>745</v>
       </c>
-      <c r="G11" s="45" t="s">
+      <c r="G11" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H11" s="45" t="s">
+      <c r="H11" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B12" s="45" t="s">
+      <c r="I11" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J11" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K11" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" s="43" t="s">
         <v>716</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="19" t="s">
         <v>582</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="19" t="s">
         <v>794</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B13" s="45" t="s">
+      <c r="I12" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J12" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" s="43" t="s">
         <v>717</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="19" t="s">
         <v>748</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="19" t="s">
         <v>747</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H13" s="45" t="s">
+      <c r="H13" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B14" s="45" t="s">
+      <c r="I13" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J13" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="43" t="s">
         <v>718</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="19" t="s">
         <v>583</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="19" t="s">
         <v>750</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="43" t="s">
         <v>795</v>
       </c>
-      <c r="H14" s="45" t="s">
+      <c r="H14" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" s="45" t="s">
+      <c r="I14" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" s="43" t="s">
         <v>719</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="19" t="s">
         <v>752</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="43" t="s">
         <v>795</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" s="45" t="s">
+      <c r="I15" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="43" t="s">
         <v>720</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="19" t="s">
         <v>584</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="19" t="s">
         <v>751</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="43" t="s">
         <v>768</v>
       </c>
-      <c r="H16" s="45" t="s">
+      <c r="H16" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B17" s="45" t="s">
+      <c r="I16" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" s="43" t="s">
         <v>721</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="19" t="s">
         <v>749</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="19" t="s">
         <v>753</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="43" t="s">
         <v>768</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="45" t="s">
+      <c r="I17" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="43" t="s">
         <v>722</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="19" t="s">
         <v>586</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="19" t="s">
         <v>754</v>
       </c>
-      <c r="G18" s="45" t="s">
+      <c r="G18" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H18" s="45" t="s">
+      <c r="H18" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="45" t="s">
+      <c r="I18" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J18" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K18" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="43" t="s">
         <v>723</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="19" t="s">
         <v>585</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="19" t="s">
         <v>755</v>
       </c>
-      <c r="G19" s="45" t="s">
+      <c r="G19" s="43" t="s">
         <v>746</v>
       </c>
-      <c r="H19" s="45" t="s">
+      <c r="H19" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B20" s="45" t="s">
+      <c r="I19" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J19" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K19" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>724</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="19" t="s">
         <v>797</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="19" t="s">
         <v>798</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="43" t="s">
         <v>770</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B21" s="45" t="s">
+      <c r="I20" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J20" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" s="43" t="s">
         <v>725</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="19" t="s">
         <v>587</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="19" t="s">
         <v>756</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="43" t="s">
         <v>799</v>
       </c>
-      <c r="H21" s="45" t="s">
+      <c r="H21" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22" s="45" t="s">
+      <c r="I21" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J21" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K21" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="43" t="s">
         <v>726</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="19" t="s">
         <v>588</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="19" t="s">
         <v>757</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="43" t="s">
         <v>769</v>
       </c>
-      <c r="H22" s="45" t="s">
+      <c r="H22" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B23" s="45" t="s">
+      <c r="I22" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J22" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K22" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B23" s="43" t="s">
         <v>727</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="19" t="s">
         <v>589</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="19" t="s">
         <v>800</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="43" t="s">
         <v>771</v>
       </c>
-      <c r="H23" s="45" t="s">
+      <c r="H23" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B24" s="45" t="s">
+      <c r="I23" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J23" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K23" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" s="43" t="s">
         <v>728</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="19" t="s">
         <v>590</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="19" t="s">
         <v>758</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="43" t="s">
         <v>772</v>
       </c>
-      <c r="H24" s="45" t="s">
+      <c r="H24" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B25" s="45" t="s">
+      <c r="I24" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J24" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K24" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B25" s="43" t="s">
         <v>729</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="19" t="s">
         <v>801</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="19" t="s">
         <v>759</v>
       </c>
-      <c r="G25" s="45" t="s">
+      <c r="G25" s="43" t="s">
         <v>773</v>
       </c>
-      <c r="H25" s="45" t="s">
+      <c r="H25" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" s="45" t="s">
+      <c r="I25" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K25" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B26" s="43" t="s">
         <v>730</v>
       </c>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="19" t="s">
         <v>802</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="19" t="s">
         <v>803</v>
       </c>
-      <c r="G26" s="45" t="s">
+      <c r="G26" s="43" t="s">
         <v>774</v>
       </c>
-      <c r="H26" s="45" t="s">
+      <c r="H26" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27" s="45" t="s">
+      <c r="I26" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J26" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K26" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="43" t="s">
         <v>731</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C27" s="19" t="s">
         <v>591</v>
       </c>
-      <c r="D27" s="42" t="s">
+      <c r="D27" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E27" s="42" t="s">
+      <c r="E27" s="19" t="s">
         <v>760</v>
       </c>
-      <c r="G27" s="45" t="s">
+      <c r="G27" s="43" t="s">
         <v>775</v>
       </c>
-      <c r="H27" s="45" t="s">
+      <c r="H27" s="43" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B28" s="45" t="s">
+      <c r="I27" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J27" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K27" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B28" s="43" t="s">
         <v>732</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="19" t="s">
         <v>592</v>
       </c>
-      <c r="D28" s="42" t="s">
+      <c r="D28" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="42" t="s">
+      <c r="E28" s="19" t="s">
         <v>761</v>
       </c>
-      <c r="G28" s="45" t="s">
+      <c r="G28" s="43" t="s">
         <v>777</v>
       </c>
-      <c r="H28" s="45" t="s">
+      <c r="H28" s="43" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="45" t="s">
+      <c r="I28" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K28" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="43" t="s">
         <v>733</v>
       </c>
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="19" t="s">
         <v>593</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D29" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E29" s="42" t="s">
+      <c r="E29" s="19" t="s">
         <v>762</v>
       </c>
-      <c r="G29" s="45" t="s">
+      <c r="G29" s="43" t="s">
         <v>778</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="H29" s="43" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="86.4" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B30" s="45" t="s">
+      <c r="I29" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J29" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K29" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="86.4" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="43" t="s">
         <v>734</v>
       </c>
-      <c r="C30" s="43" t="s">
+      <c r="C30" s="19" t="s">
         <v>594</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="19" t="s">
         <v>804</v>
       </c>
-      <c r="G30" s="45" t="s">
+      <c r="G30" s="43" t="s">
         <v>805</v>
       </c>
-      <c r="H30" s="45" t="s">
+      <c r="H30" s="43" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="57.6" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B31" s="45" t="s">
+      <c r="I30" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J30" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K30" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="43" t="s">
         <v>735</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C31" s="19" t="s">
         <v>595</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="19" t="s">
         <v>807</v>
       </c>
-      <c r="G31" s="45" t="s">
+      <c r="G31" s="43" t="s">
         <v>782</v>
       </c>
-      <c r="H31" s="45" t="s">
+      <c r="H31" s="43" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B32" s="45" t="s">
+      <c r="I31" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" s="43" t="s">
         <v>736</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="19" t="s">
         <v>596</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="19" t="s">
         <v>763</v>
       </c>
-      <c r="G32" s="45" t="s">
+      <c r="G32" s="43" t="s">
         <v>781</v>
       </c>
-      <c r="H32" s="45" t="s">
+      <c r="H32" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="45" t="s">
+      <c r="I32" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J32" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K32" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B33" s="43" t="s">
         <v>737</v>
       </c>
-      <c r="C33" s="44" t="s">
+      <c r="C33" s="45" t="s">
         <v>597</v>
       </c>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="19" t="s">
         <v>764</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="43" t="s">
         <v>784</v>
       </c>
-      <c r="H33" s="45" t="s">
+      <c r="H33" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B34" s="45" t="s">
+      <c r="I33" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J33" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K33" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" s="43" t="s">
         <v>738</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="45" t="s">
         <v>808</v>
       </c>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="19" t="s">
         <v>765</v>
       </c>
-      <c r="G34" s="45" t="s">
+      <c r="G34" s="43" t="s">
         <v>785</v>
       </c>
-      <c r="H34" s="45" t="s">
+      <c r="H34" s="43" t="s">
         <v>786</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B35" s="45" t="s">
+      <c r="I34" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J34" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K34" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="43" t="s">
         <v>739</v>
       </c>
-      <c r="C35" s="44" t="s">
+      <c r="C35" s="45" t="s">
         <v>598</v>
       </c>
-      <c r="D35" s="42" t="s">
+      <c r="D35" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="42" t="s">
+      <c r="E35" s="19" t="s">
         <v>766</v>
       </c>
-      <c r="G35" s="45" t="s">
+      <c r="G35" s="43" t="s">
         <v>787</v>
       </c>
-      <c r="H35" s="45" t="s">
+      <c r="H35" s="43" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="28.8" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B36" s="45" t="s">
+      <c r="I35" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J35" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K35" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="28.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" s="43" t="s">
         <v>740</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C36" s="45" t="s">
         <v>599</v>
       </c>
-      <c r="D36" s="42" t="s">
+      <c r="D36" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="42" t="s">
+      <c r="E36" s="19" t="s">
         <v>767</v>
       </c>
-      <c r="G36" s="45" t="s">
+      <c r="G36" s="43" t="s">
         <v>789</v>
       </c>
-      <c r="H36" s="45" t="s">
+      <c r="H36" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B37" s="45" t="s">
+      <c r="I36" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J36" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K36" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="43" t="s">
         <v>741</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="42" t="s">
+      <c r="E37" s="19" t="s">
         <v>810</v>
       </c>
-      <c r="G37" s="45" t="s">
+      <c r="G37" s="43" t="s">
         <v>790</v>
       </c>
-      <c r="H37" s="45" t="s">
+      <c r="H37" s="43" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="43.2" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="B38" s="45" t="s">
+      <c r="I37" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J37" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K37" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B38" s="43" t="s">
         <v>742</v>
       </c>
-      <c r="C38" s="44" t="s">
+      <c r="C38" s="45" t="s">
         <v>600</v>
       </c>
-      <c r="D38" s="42" t="s">
+      <c r="D38" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="42" t="s">
+      <c r="E38" s="19" t="s">
         <v>809</v>
       </c>
-      <c r="G38" s="45" t="s">
+      <c r="G38" s="43" t="s">
         <v>791</v>
       </c>
-      <c r="H38" s="45" t="s">
+      <c r="H38" s="43" t="s">
         <v>744</v>
       </c>
+      <c r="I38" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J38" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K38" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" s="43" t="s">
+        <v>826</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>823</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>932</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H39" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I39" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J39" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K39" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>827</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>975</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>933</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H40" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I40" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J40" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K40" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>828</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>824</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>934</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H41" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I41" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J41" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K41" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>829</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>825</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>936</v>
+      </c>
+      <c r="G42" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H42" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I42" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J42" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K42" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>830</v>
+      </c>
+      <c r="C43" s="45" t="s">
+        <v>851</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>937</v>
+      </c>
+      <c r="G43" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I43" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J43" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K43" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>831</v>
+      </c>
+      <c r="C44" s="45" t="s">
+        <v>852</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>938</v>
+      </c>
+      <c r="G44" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H44" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I44" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J44" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K44" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>832</v>
+      </c>
+      <c r="C45" s="45" t="s">
+        <v>853</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="G45" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H45" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I45" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J45" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K45" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>833</v>
+      </c>
+      <c r="C46" s="45" t="s">
+        <v>854</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>935</v>
+      </c>
+      <c r="G46" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I46" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J46" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K46" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>834</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>856</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>939</v>
+      </c>
+      <c r="G47" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I47" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J47" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K47" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>835</v>
+      </c>
+      <c r="C48" s="45" t="s">
+        <v>855</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>940</v>
+      </c>
+      <c r="G48" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I48" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J48" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K48" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>836</v>
+      </c>
+      <c r="C49" s="45" t="s">
+        <v>867</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>941</v>
+      </c>
+      <c r="G49" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H49" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I49" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J49" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K49" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>837</v>
+      </c>
+      <c r="C50" s="45" t="s">
+        <v>977</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>942</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H50" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I50" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J50" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K50" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>838</v>
+      </c>
+      <c r="C51" s="45" t="s">
+        <v>857</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>943</v>
+      </c>
+      <c r="G51" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H51" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I51" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J51" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K51" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>839</v>
+      </c>
+      <c r="C52" s="45" t="s">
+        <v>858</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>945</v>
+      </c>
+      <c r="G52" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H52" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I52" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J52" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K52" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>840</v>
+      </c>
+      <c r="C53" s="45" t="s">
+        <v>859</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>944</v>
+      </c>
+      <c r="G53" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H53" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I53" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J53" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K53" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="43" t="s">
+        <v>841</v>
+      </c>
+      <c r="C54" s="45" t="s">
+        <v>860</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>946</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I54" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J54" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K54" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>842</v>
+      </c>
+      <c r="C55" s="45" t="s">
+        <v>861</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>947</v>
+      </c>
+      <c r="G55" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H55" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I55" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J55" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K55" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>843</v>
+      </c>
+      <c r="C56" s="45" t="s">
+        <v>978</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>948</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H56" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I56" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J56" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K56" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>844</v>
+      </c>
+      <c r="C57" s="45" t="s">
+        <v>862</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>949</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H57" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I57" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J57" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K57" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="43" t="s">
+        <v>845</v>
+      </c>
+      <c r="C58" s="45" t="s">
+        <v>863</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>954</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H58" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I58" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J58" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K58" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="43" t="s">
+        <v>846</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>864</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>953</v>
+      </c>
+      <c r="G59" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H59" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I59" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J59" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K59" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B60" s="43" t="s">
+        <v>847</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>865</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>951</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H60" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I60" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J60" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K60" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" s="43" t="s">
+        <v>848</v>
+      </c>
+      <c r="C61" s="45" t="s">
+        <v>866</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>950</v>
+      </c>
+      <c r="G61" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H61" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I61" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J61" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K61" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62" s="43" t="s">
+        <v>849</v>
+      </c>
+      <c r="C62" s="45" t="s">
+        <v>868</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>955</v>
+      </c>
+      <c r="G62" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H62" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I62" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J62" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K62" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B63" s="43" t="s">
+        <v>850</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>869</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>956</v>
+      </c>
+      <c r="G63" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H63" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I63" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J63" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K63" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>871</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>870</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>957</v>
+      </c>
+      <c r="G64" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H64" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I64" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J64" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K64" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B65" s="43" t="s">
+        <v>883</v>
+      </c>
+      <c r="C65" s="45" t="s">
+        <v>872</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>958</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H65" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I65" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J65" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K65" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="43" t="s">
+        <v>884</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>873</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>959</v>
+      </c>
+      <c r="G66" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H66" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I66" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J66" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K66" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B67" s="43" t="s">
+        <v>885</v>
+      </c>
+      <c r="C67" s="45" t="s">
+        <v>875</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>960</v>
+      </c>
+      <c r="G67" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H67" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I67" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J67" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K67" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B68" s="43" t="s">
+        <v>886</v>
+      </c>
+      <c r="C68" s="45" t="s">
+        <v>874</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>961</v>
+      </c>
+      <c r="G68" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H68" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I68" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J68" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K68" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B69" s="43" t="s">
+        <v>887</v>
+      </c>
+      <c r="C69" s="45" t="s">
+        <v>876</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>963</v>
+      </c>
+      <c r="G69" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H69" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I69" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J69" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K69" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B70" s="43" t="s">
+        <v>888</v>
+      </c>
+      <c r="C70" s="45" t="s">
+        <v>877</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>962</v>
+      </c>
+      <c r="G70" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H70" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I70" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J70" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K70" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71" s="43" t="s">
+        <v>889</v>
+      </c>
+      <c r="C71" s="45" t="s">
+        <v>878</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>952</v>
+      </c>
+      <c r="G71" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H71" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I71" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J71" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K71" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B72" s="43" t="s">
+        <v>890</v>
+      </c>
+      <c r="C72" s="45" t="s">
+        <v>979</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>964</v>
+      </c>
+      <c r="G72" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H72" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I72" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J72" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K72" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B73" s="43" t="s">
+        <v>891</v>
+      </c>
+      <c r="C73" s="45" t="s">
+        <v>879</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>965</v>
+      </c>
+      <c r="G73" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H73" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I73" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J73" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K73" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="43" t="s">
+        <v>892</v>
+      </c>
+      <c r="C74" s="45" t="s">
+        <v>880</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>968</v>
+      </c>
+      <c r="G74" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H74" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I74" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J74" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K74" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B75" s="43" t="s">
+        <v>893</v>
+      </c>
+      <c r="C75" s="45" t="s">
+        <v>881</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>966</v>
+      </c>
+      <c r="G75" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H75" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I75" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J75" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K75" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="B76" s="43" t="s">
+        <v>894</v>
+      </c>
+      <c r="C76" s="45" t="s">
+        <v>882</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>967</v>
+      </c>
+      <c r="G76" s="44" t="s">
+        <v>746</v>
+      </c>
+      <c r="H76" s="43" t="s">
+        <v>744</v>
+      </c>
+      <c r="I76" s="44" t="s">
+        <v>153</v>
+      </c>
+      <c r="J76" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="K76" s="43" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="36" customFormat="1" ht="22.2" customHeight="1" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="36" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B78" s="43" t="s">
+        <v>813</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>814</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>969</v>
+      </c>
+      <c r="G78" s="19" t="s">
+        <v>971</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>972</v>
+      </c>
+      <c r="I78" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J78" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K78" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B79" s="43" t="s">
+        <v>906</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>815</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>970</v>
+      </c>
+      <c r="G79" s="19" t="s">
+        <v>971</v>
+      </c>
+      <c r="H79" s="19" t="s">
+        <v>972</v>
+      </c>
+      <c r="I79" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J79" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K79" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B80" s="43" t="s">
+        <v>907</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>816</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>980</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>981</v>
+      </c>
+      <c r="H80" s="19" t="s">
+        <v>982</v>
+      </c>
+      <c r="I80" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J80" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K80" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="72" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B81" s="43" t="s">
+        <v>908</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>973</v>
+      </c>
+      <c r="D81" s="19" t="s">
+        <v>983</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>984</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>985</v>
+      </c>
+      <c r="H81" s="19" t="s">
+        <v>986</v>
+      </c>
+      <c r="I81" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J81" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K81" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" ht="57.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B82" s="43" t="s">
+        <v>909</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>983</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>987</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>988</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>989</v>
+      </c>
+      <c r="I82" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J82" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K82" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="42" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B83" s="43" t="s">
+        <v>910</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>974</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>983</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G83" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H83" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I83" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J83" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K83" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="67.8" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B84" s="43" t="s">
+        <v>911</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>818</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>994</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>995</v>
+      </c>
+      <c r="H84" s="19" t="s">
+        <v>996</v>
+      </c>
+      <c r="I84" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J84" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K84" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B85" s="43" t="s">
+        <v>912</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>819</v>
+      </c>
+      <c r="D85" s="19" t="s">
+        <v>997</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>998</v>
+      </c>
+      <c r="G85" s="19" t="s">
+        <v>1024</v>
+      </c>
+      <c r="H85" s="19" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I85" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J85" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K85" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="37.799999999999997" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B86" s="43" t="s">
+        <v>913</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D86" s="19" t="s">
+        <v>999</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G86" s="19" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H86" s="19" t="s">
+        <v>1027</v>
+      </c>
+      <c r="I86" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J86" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K86" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="43.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B87" s="43" t="s">
+        <v>914</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>820</v>
+      </c>
+      <c r="D87" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G87" s="19" t="s">
+        <v>1003</v>
+      </c>
+      <c r="H87" s="19" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I87" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J87" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K87" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="48.6" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B88" s="43" t="s">
+        <v>915</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>821</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H88" s="19" t="s">
+        <v>1006</v>
+      </c>
+      <c r="I88" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J88" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K88" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="64.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B89" s="43" t="s">
+        <v>916</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>822</v>
+      </c>
+      <c r="D89" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E89" s="19" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="H89" s="19" t="s">
+        <v>744</v>
+      </c>
+      <c r="I89" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J89" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K89" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B90" s="43" t="s">
+        <v>917</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>895</v>
+      </c>
+      <c r="D90" s="19" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G90" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H90" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I90" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J90" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K90" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B91" s="43" t="s">
+        <v>918</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>896</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G91" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H91" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I91" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J91" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K91" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B92" s="43" t="s">
+        <v>919</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>897</v>
+      </c>
+      <c r="D92" s="19" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G92" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H92" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I92" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J92" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K92" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B93" s="43" t="s">
+        <v>920</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>898</v>
+      </c>
+      <c r="D93" s="19" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G93" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H93" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I93" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J93" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K93" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B94" s="43" t="s">
+        <v>921</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>901</v>
+      </c>
+      <c r="D94" s="19" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G94" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H94" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I94" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J94" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K94" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B95" s="43" t="s">
+        <v>922</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>902</v>
+      </c>
+      <c r="D95" s="19" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E95" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G95" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H95" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I95" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J95" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K95" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B96" s="43" t="s">
+        <v>923</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>903</v>
+      </c>
+      <c r="D96" s="19" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G96" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H96" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I96" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J96" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K96" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B97" s="43" t="s">
+        <v>924</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>904</v>
+      </c>
+      <c r="D97" s="19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E97" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G97" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H97" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I97" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J97" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K97" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B98" s="43" t="s">
+        <v>925</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>905</v>
+      </c>
+      <c r="D98" s="19" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E98" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G98" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H98" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I98" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J98" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K98" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B99" s="43" t="s">
+        <v>926</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>899</v>
+      </c>
+      <c r="D99" s="19" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="G99" s="19" t="s">
+        <v>991</v>
+      </c>
+      <c r="H99" s="19" t="s">
+        <v>992</v>
+      </c>
+      <c r="I99" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J99" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K99" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="38.4" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B100" s="43" t="s">
+        <v>927</v>
+      </c>
+      <c r="C100" s="19" t="s">
+        <v>900</v>
+      </c>
+      <c r="D100" s="19" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E100" s="19" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G100" s="19" t="s">
+        <v>1029</v>
+      </c>
+      <c r="H100" s="19" t="s">
+        <v>1030</v>
+      </c>
+      <c r="I100" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J100" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K100" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="45.6" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B101" s="43" t="s">
+        <v>928</v>
+      </c>
+      <c r="C101" s="19" t="s">
+        <v>930</v>
+      </c>
+      <c r="D101" s="19" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E101" s="19" t="s">
+        <v>1021</v>
+      </c>
+      <c r="G101" s="19" t="s">
+        <v>1031</v>
+      </c>
+      <c r="H101" s="19" t="s">
+        <v>1032</v>
+      </c>
+      <c r="I101" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J101" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K101" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="22.2" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>929</v>
+      </c>
+      <c r="C102" s="19" t="s">
+        <v>931</v>
+      </c>
+      <c r="D102" s="19" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E102" s="19" t="s">
+        <v>1023</v>
+      </c>
+      <c r="G102" s="19" t="s">
+        <v>1033</v>
+      </c>
+      <c r="H102" s="19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I102" s="44" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J102" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="K102" s="44" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="A7:XFD7"/>
     <mergeCell ref="A8:XFD8"/>
+    <mergeCell ref="A77:XFD77"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>